<commit_message>
Update SubRES Excel templates
Replace two SubRES workbook files with updated versions: SubRES_TMPL/SubRES_2.0_ELC_NREL-ATB-2021.xlsm and SubRES_TMPL/SubRes_2.1_ELC_EIA_AEO2022.xlsx. Simplify the SubRES calibration particularly for Solar capacity factors for now.
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRes_2.1_ELC_EIA_AEO2022.xlsx
+++ b/SubRES_TMPL/SubRes_2.1_ELC_EIA_AEO2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\esma\OTAI\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\esma\DEVTAI\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758D7DCD-E9E0-45DA-B801-CB30EBBA73EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FC2A41-E44A-41CA-B24A-F03307B19DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38775" yWindow="1065" windowWidth="33075" windowHeight="17910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51960" yWindow="5535" windowWidth="57600" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC_NEW_GENERATORS" sheetId="1" r:id="rId1"/>
@@ -1372,13 +1372,13 @@
   <dimension ref="A1:AP95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB12" sqref="AB12"/>
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="79.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -1386,7 +1386,7 @@
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="1.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="79.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -1401,14 +1401,13 @@
     <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.140625" customWidth="1"/>
+    <col min="27" max="28" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="21" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="21" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="34.140625" bestFit="1" customWidth="1"/>
@@ -1630,11 +1629,11 @@
         <v>17</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B27" si="0">"E_"&amp;AI4&amp;"_"&amp;AJ4&amp;"_"&amp;AL4</f>
-        <v>E_COA_CAV_01</v>
+        <f>"E_"&amp;AH4&amp;"_"&amp;AI4&amp;"_"&amp;AJ4&amp;"_"&amp;AL4</f>
+        <v>E_THM_COA_CAV_01</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C26" si="1">AK4&amp;"_"&amp;AG4</f>
+        <f t="shared" ref="C4:C26" si="0">AK4&amp;"_"&amp;AG4</f>
         <v>Electricity Power Plant_Ultra-supercritical coal (USC)</v>
       </c>
       <c r="D4" t="s">
@@ -1647,15 +1646,15 @@
         <v>20</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:K20" si="2">B4</f>
-        <v>E_COA_CAV_01</v>
+        <f t="shared" ref="K4:K20" si="1">B4</f>
+        <v>E_THM_COA_CAV_01</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:L20" si="3">C4</f>
+        <f t="shared" ref="L4:L20" si="2">C4</f>
         <v>Electricity Power Plant_Ultra-supercritical coal (USC)</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" ref="M4:M17" si="4">"ELC"&amp;AI4</f>
+        <f t="shared" ref="M4:M17" si="3">"ELC"&amp;AI4</f>
         <v>ELCCOA</v>
       </c>
       <c r="N4" t="s">
@@ -1735,11 +1734,11 @@
         <v>17</v>
       </c>
       <c r="B5" t="str">
+        <f t="shared" ref="B5:B27" si="4">"E_"&amp;AH5&amp;"_"&amp;AI5&amp;"_"&amp;AJ5&amp;"_"&amp;AL5</f>
+        <v>E_THM_COA_COQ_01</v>
+      </c>
+      <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>E_COA_COQ_01</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant with CCS_USC with 30% carbon capture and sequestration (CCS)</v>
       </c>
       <c r="D5" t="s">
@@ -1752,15 +1751,15 @@
         <v>20</v>
       </c>
       <c r="K5" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_COA_COQ_01</v>
+      </c>
+      <c r="L5" t="str">
         <f t="shared" si="2"/>
-        <v>E_COA_COQ_01</v>
-      </c>
-      <c r="L5" t="str">
+        <v>Electricity Power Plant with CCS_USC with 30% carbon capture and sequestration (CCS)</v>
+      </c>
+      <c r="M5" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant with CCS_USC with 30% carbon capture and sequestration (CCS)</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" si="4"/>
         <v>ELCCOA</v>
       </c>
       <c r="N5" t="s">
@@ -1840,11 +1839,11 @@
         <v>17</v>
       </c>
       <c r="B6" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_COA_COQ_01</v>
+      </c>
+      <c r="C6" t="str">
         <f t="shared" si="0"/>
-        <v>E_COA_COQ_01</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant with CCS_USC with 90% CCS</v>
       </c>
       <c r="D6" t="s">
@@ -1857,15 +1856,15 @@
         <v>20</v>
       </c>
       <c r="K6" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_COA_COQ_01</v>
+      </c>
+      <c r="L6" t="str">
         <f t="shared" si="2"/>
-        <v>E_COA_COQ_01</v>
-      </c>
-      <c r="L6" t="str">
+        <v>Electricity Power Plant with CCS_USC with 90% CCS</v>
+      </c>
+      <c r="M6" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant with CCS_USC with 90% CCS</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" si="4"/>
         <v>ELCCOA</v>
       </c>
       <c r="N6" t="s">
@@ -1945,11 +1944,11 @@
         <v>17</v>
       </c>
       <c r="B7" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_NGA_CCG_01</v>
+      </c>
+      <c r="C7" t="str">
         <f t="shared" si="0"/>
-        <v>E_NGA_CCG_01</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Combined-cycle—single shaft</v>
       </c>
       <c r="D7" t="s">
@@ -1962,15 +1961,15 @@
         <v>20</v>
       </c>
       <c r="K7" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_NGA_CCG_01</v>
+      </c>
+      <c r="L7" t="str">
         <f t="shared" si="2"/>
-        <v>E_NGA_CCG_01</v>
-      </c>
-      <c r="L7" t="str">
+        <v>Electricity Power Plant_Combined-cycle—single shaft</v>
+      </c>
+      <c r="M7" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant_Combined-cycle—single shaft</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" si="4"/>
         <v>ELCNGA</v>
       </c>
       <c r="N7" t="s">
@@ -2050,11 +2049,11 @@
         <v>17</v>
       </c>
       <c r="B8" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_NGA_CCG_01</v>
+      </c>
+      <c r="C8" t="str">
         <f t="shared" si="0"/>
-        <v>E_NGA_CCG_01</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Combined-cycle—multi shaft</v>
       </c>
       <c r="D8" t="s">
@@ -2067,15 +2066,15 @@
         <v>20</v>
       </c>
       <c r="K8" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_NGA_CCG_01</v>
+      </c>
+      <c r="L8" t="str">
         <f t="shared" si="2"/>
-        <v>E_NGA_CCG_01</v>
-      </c>
-      <c r="L8" t="str">
+        <v>Electricity Power Plant_Combined-cycle—multi shaft</v>
+      </c>
+      <c r="M8" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant_Combined-cycle—multi shaft</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" si="4"/>
         <v>ELCNGA</v>
       </c>
       <c r="N8" t="s">
@@ -2155,11 +2154,11 @@
         <v>17</v>
       </c>
       <c r="B9" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_NGA_ACS_01</v>
+      </c>
+      <c r="C9" t="str">
         <f t="shared" si="0"/>
-        <v>E_NGA_ACS_01</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant with CCS_Combined-cycle with 90% CCS</v>
       </c>
       <c r="D9" t="s">
@@ -2172,15 +2171,15 @@
         <v>20</v>
       </c>
       <c r="K9" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_NGA_ACS_01</v>
+      </c>
+      <c r="L9" t="str">
         <f t="shared" si="2"/>
-        <v>E_NGA_ACS_01</v>
-      </c>
-      <c r="L9" t="str">
+        <v>Electricity Power Plant with CCS_Combined-cycle with 90% CCS</v>
+      </c>
+      <c r="M9" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant with CCS_Combined-cycle with 90% CCS</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" si="4"/>
         <v>ELCNGA</v>
       </c>
       <c r="N9" t="s">
@@ -2260,11 +2259,11 @@
         <v>17</v>
       </c>
       <c r="B10" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_NGA_ICE_01</v>
+      </c>
+      <c r="C10" t="str">
         <f t="shared" si="0"/>
-        <v>E_NGA_ICE_01</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Internal combustion engine</v>
       </c>
       <c r="D10" t="s">
@@ -2277,15 +2276,15 @@
         <v>20</v>
       </c>
       <c r="K10" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_NGA_ICE_01</v>
+      </c>
+      <c r="L10" t="str">
         <f t="shared" si="2"/>
-        <v>E_NGA_ICE_01</v>
-      </c>
-      <c r="L10" t="str">
+        <v>Electricity Power Plant_Internal combustion engine</v>
+      </c>
+      <c r="M10" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant_Internal combustion engine</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" si="4"/>
         <v>ELCNGA</v>
       </c>
       <c r="N10" t="s">
@@ -2365,11 +2364,11 @@
         <v>17</v>
       </c>
       <c r="B11" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_NGA_CTA_01</v>
+      </c>
+      <c r="C11" t="str">
         <f t="shared" si="0"/>
-        <v>E_NGA_CTA_01</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Combustion turbine—aeroderivative</v>
       </c>
       <c r="D11" t="s">
@@ -2382,15 +2381,15 @@
         <v>20</v>
       </c>
       <c r="K11" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_NGA_CTA_01</v>
+      </c>
+      <c r="L11" t="str">
         <f t="shared" si="2"/>
-        <v>E_NGA_CTA_01</v>
-      </c>
-      <c r="L11" t="str">
+        <v>Electricity Power Plant_Combustion turbine—aeroderivative</v>
+      </c>
+      <c r="M11" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant_Combustion turbine—aeroderivative</v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" si="4"/>
         <v>ELCNGA</v>
       </c>
       <c r="N11" t="s">
@@ -2470,11 +2469,11 @@
         <v>17</v>
       </c>
       <c r="B12" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_NGA_ACT_01</v>
+      </c>
+      <c r="C12" t="str">
         <f t="shared" si="0"/>
-        <v>E_NGA_ACT_01</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Combustion turbine—industrial frame</v>
       </c>
       <c r="D12" t="s">
@@ -2487,15 +2486,15 @@
         <v>20</v>
       </c>
       <c r="K12" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_NGA_ACT_01</v>
+      </c>
+      <c r="L12" t="str">
         <f t="shared" si="2"/>
-        <v>E_NGA_ACT_01</v>
-      </c>
-      <c r="L12" t="str">
+        <v>Electricity Power Plant_Combustion turbine—industrial frame</v>
+      </c>
+      <c r="M12" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant_Combustion turbine—industrial frame</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" si="4"/>
         <v>ELCNGA</v>
       </c>
       <c r="N12" t="s">
@@ -2575,11 +2574,11 @@
         <v>17</v>
       </c>
       <c r="B13" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_H2_FCG_01</v>
+      </c>
+      <c r="C13" t="str">
         <f t="shared" si="0"/>
-        <v>E_H2_FCG_01</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Fuel cells</v>
       </c>
       <c r="D13" t="s">
@@ -2592,15 +2591,15 @@
         <v>20</v>
       </c>
       <c r="K13" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_H2_FCG_01</v>
+      </c>
+      <c r="L13" t="str">
         <f t="shared" si="2"/>
-        <v>E_H2_FCG_01</v>
-      </c>
-      <c r="L13" t="str">
+        <v>Electricity Power Plant_Fuel cells</v>
+      </c>
+      <c r="M13" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant_Fuel cells</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" si="4"/>
         <v>ELCH2</v>
       </c>
       <c r="N13" t="s">
@@ -2680,11 +2679,11 @@
         <v>17</v>
       </c>
       <c r="B14" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_NUC_CNU_01</v>
+      </c>
+      <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v>E_NUC_CNU_01</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Nuclear—light water reactor</v>
       </c>
       <c r="D14" t="s">
@@ -2697,15 +2696,15 @@
         <v>20</v>
       </c>
       <c r="K14" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_NUC_CNU_01</v>
+      </c>
+      <c r="L14" t="str">
         <f t="shared" si="2"/>
-        <v>E_NUC_CNU_01</v>
-      </c>
-      <c r="L14" t="str">
+        <v>Electricity Power Plant_Nuclear—light water reactor</v>
+      </c>
+      <c r="M14" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant_Nuclear—light water reactor</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="4"/>
         <v>ELCNUC</v>
       </c>
       <c r="N14" t="s">
@@ -2785,11 +2784,11 @@
         <v>17</v>
       </c>
       <c r="B15" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_NUC_SMR_01</v>
+      </c>
+      <c r="C15" t="str">
         <f t="shared" si="0"/>
-        <v>E_NUC_SMR_01</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Nuclear—small modular reactor</v>
       </c>
       <c r="D15" t="s">
@@ -2802,15 +2801,15 @@
         <v>20</v>
       </c>
       <c r="K15" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_NUC_SMR_01</v>
+      </c>
+      <c r="L15" t="str">
         <f t="shared" si="2"/>
-        <v>E_NUC_SMR_01</v>
-      </c>
-      <c r="L15" t="str">
+        <v>Electricity Power Plant_Nuclear—small modular reactor</v>
+      </c>
+      <c r="M15" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant_Nuclear—small modular reactor</v>
-      </c>
-      <c r="M15" t="str">
-        <f t="shared" si="4"/>
         <v>ELCNUC</v>
       </c>
       <c r="N15" t="s">
@@ -2890,11 +2889,11 @@
         <v>17</v>
       </c>
       <c r="B16" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_OTH_DGB_01</v>
+      </c>
+      <c r="C16" t="str">
         <f t="shared" si="0"/>
-        <v>E_OTH_DGB_01</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Distributed generation—base</v>
       </c>
       <c r="D16" t="s">
@@ -2907,15 +2906,15 @@
         <v>20</v>
       </c>
       <c r="K16" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_OTH_DGB_01</v>
+      </c>
+      <c r="L16" t="str">
         <f t="shared" si="2"/>
-        <v>E_OTH_DGB_01</v>
-      </c>
-      <c r="L16" t="str">
+        <v>Electricity Power Plant_Distributed generation—base</v>
+      </c>
+      <c r="M16" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant_Distributed generation—base</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" si="4"/>
         <v>ELCOTH</v>
       </c>
       <c r="N16" t="s">
@@ -2995,11 +2994,11 @@
         <v>17</v>
       </c>
       <c r="B17" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_OTH_DGP_01</v>
+      </c>
+      <c r="C17" t="str">
         <f t="shared" si="0"/>
-        <v>E_OTH_DGP_01</v>
-      </c>
-      <c r="C17" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Distributed generation—peak</v>
       </c>
       <c r="D17" t="s">
@@ -3012,15 +3011,15 @@
         <v>20</v>
       </c>
       <c r="K17" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_OTH_DGP_01</v>
+      </c>
+      <c r="L17" t="str">
         <f t="shared" si="2"/>
-        <v>E_OTH_DGP_01</v>
-      </c>
-      <c r="L17" t="str">
+        <v>Electricity Power Plant_Distributed generation—peak</v>
+      </c>
+      <c r="M17" t="str">
         <f t="shared" si="3"/>
-        <v>Electricity Power Plant_Distributed generation—peak</v>
-      </c>
-      <c r="M17" t="str">
-        <f t="shared" si="4"/>
         <v>ELCOTH</v>
       </c>
       <c r="N17" t="s">
@@ -3100,11 +3099,11 @@
         <v>106</v>
       </c>
       <c r="B18" t="str">
+        <f t="shared" si="4"/>
+        <v>E_STG_ELCC_QST_01</v>
+      </c>
+      <c r="C18" t="str">
         <f t="shared" si="0"/>
-        <v>E_ELCC_QST_01</v>
-      </c>
-      <c r="C18" t="str">
-        <f t="shared" si="1"/>
         <v>Storage_Battery storage</v>
       </c>
       <c r="D18" t="s">
@@ -3117,11 +3116,11 @@
         <v>20</v>
       </c>
       <c r="K18" t="str">
+        <f t="shared" si="1"/>
+        <v>E_STG_ELCC_QST_01</v>
+      </c>
+      <c r="L18" t="str">
         <f t="shared" si="2"/>
-        <v>E_ELCC_QST_01</v>
-      </c>
-      <c r="L18" t="str">
-        <f t="shared" si="3"/>
         <v>Storage_Battery storage</v>
       </c>
       <c r="M18" t="str">
@@ -3204,11 +3203,11 @@
         <v>17</v>
       </c>
       <c r="B19" t="str">
+        <f t="shared" si="4"/>
+        <v>E_THM_BSL_BMS_01</v>
+      </c>
+      <c r="C19" t="str">
         <f t="shared" si="0"/>
-        <v>E_BSL_BMS_01</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" si="1"/>
         <v>Electricity Power Plant_Biomass</v>
       </c>
       <c r="D19" t="s">
@@ -3221,11 +3220,11 @@
         <v>20</v>
       </c>
       <c r="K19" t="str">
+        <f t="shared" si="1"/>
+        <v>E_THM_BSL_BMS_01</v>
+      </c>
+      <c r="L19" t="str">
         <f t="shared" si="2"/>
-        <v>E_BSL_BMS_01</v>
-      </c>
-      <c r="L19" t="str">
-        <f t="shared" si="3"/>
         <v>Electricity Power Plant_Biomass</v>
       </c>
       <c r="M19" t="str">
@@ -3309,11 +3308,11 @@
         <v>17</v>
       </c>
       <c r="B20" t="str">
+        <f t="shared" si="4"/>
+        <v>E_RNW_GEO_GTH_01</v>
+      </c>
+      <c r="C20" t="str">
         <f t="shared" si="0"/>
-        <v>E_GEO_GTH_01</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="1"/>
         <v>Geothermal Plant_Geothermal</v>
       </c>
       <c r="D20" t="s">
@@ -3326,11 +3325,11 @@
         <v>20</v>
       </c>
       <c r="K20" t="str">
+        <f t="shared" si="1"/>
+        <v>E_RNW_GEO_GTH_01</v>
+      </c>
+      <c r="L20" t="str">
         <f t="shared" si="2"/>
-        <v>E_GEO_GTH_01</v>
-      </c>
-      <c r="L20" t="str">
-        <f t="shared" si="3"/>
         <v>Geothermal Plant_Geothermal</v>
       </c>
       <c r="M20" t="str">
@@ -3414,11 +3413,11 @@
         <v>17</v>
       </c>
       <c r="B21" t="str">
+        <f t="shared" si="4"/>
+        <v>E_RNW_WAT_HYC_01</v>
+      </c>
+      <c r="C21" t="str">
         <f t="shared" si="0"/>
-        <v>E_WAT_HYC_01</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="1"/>
         <v>Hydro Plant_Conventional hydropower</v>
       </c>
       <c r="D21" t="s">
@@ -3432,7 +3431,7 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" ref="K21:K27" si="6">B21</f>
-        <v>E_WAT_HYC_01</v>
+        <v>E_RNW_WAT_HYC_01</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" ref="L21:L26" si="7">C21</f>
@@ -3518,11 +3517,11 @@
         <v>17</v>
       </c>
       <c r="B22" t="str">
+        <f t="shared" si="4"/>
+        <v>E_RNW_WNO_WND_01</v>
+      </c>
+      <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>E_WNO_WND_01</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="1"/>
         <v>Wind Onshore_Wind</v>
       </c>
       <c r="D22" t="s">
@@ -3536,7 +3535,7 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="6"/>
-        <v>E_WNO_WND_01</v>
+        <v>E_RNW_WNO_WND_01</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="7"/>
@@ -3622,11 +3621,11 @@
         <v>17</v>
       </c>
       <c r="B23" t="str">
+        <f t="shared" si="4"/>
+        <v>E_RNW_WNF_WFS_01</v>
+      </c>
+      <c r="C23" t="str">
         <f t="shared" si="0"/>
-        <v>E_WNF_WFS_01</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="1"/>
         <v>Wind Offshore_Wind offshore</v>
       </c>
       <c r="D23" t="s">
@@ -3640,7 +3639,7 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="6"/>
-        <v>E_WNF_WFS_01</v>
+        <v>E_RNW_WNF_WFS_01</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="7"/>
@@ -3726,11 +3725,11 @@
         <v>17</v>
       </c>
       <c r="B24" t="str">
+        <f t="shared" si="4"/>
+        <v>E_RNW_STH_STH_01</v>
+      </c>
+      <c r="C24" t="str">
         <f t="shared" si="0"/>
-        <v>E_STH_STH_01</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="1"/>
         <v>Solar Thermal_Solar thermal</v>
       </c>
       <c r="D24" t="s">
@@ -3744,7 +3743,7 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="6"/>
-        <v>E_STH_STH_01</v>
+        <v>E_RNW_STH_STH_01</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="7"/>
@@ -3830,11 +3829,11 @@
         <v>17</v>
       </c>
       <c r="B25" t="str">
+        <f t="shared" si="4"/>
+        <v>E_RNW_SPV_SPV_01</v>
+      </c>
+      <c r="C25" t="str">
         <f t="shared" si="0"/>
-        <v>E_SPV_SPV_01</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="1"/>
         <v>Solar PV_Solar photovoltaic (PV) with tracking</v>
       </c>
       <c r="D25" t="s">
@@ -3848,7 +3847,7 @@
       </c>
       <c r="K25" t="str">
         <f t="shared" si="6"/>
-        <v>E_SPV_SPV_01</v>
+        <v>E_RNW_SPV_SPV_01</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="7"/>
@@ -3890,7 +3889,7 @@
         <v>31.536000000000001</v>
       </c>
       <c r="X25" s="1">
-        <v>0.35</v>
+        <v>0.11</v>
       </c>
       <c r="Z25">
         <f>NEMS_EMM_AEO2022!C24+1</f>
@@ -3934,11 +3933,11 @@
         <v>17</v>
       </c>
       <c r="B26" t="str">
+        <f t="shared" si="4"/>
+        <v>E_RNW_SPV_SPS_01</v>
+      </c>
+      <c r="C26" t="str">
         <f t="shared" si="0"/>
-        <v>E_SPV_SPS_01</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="1"/>
         <v>Solar PV w Storage_Solar PV with storage</v>
       </c>
       <c r="D26" t="s">
@@ -3952,7 +3951,7 @@
       </c>
       <c r="K26" t="str">
         <f t="shared" si="6"/>
-        <v>E_SPV_SPS_01</v>
+        <v>E_RNW_SPV_SPS_01</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="7"/>
@@ -3994,7 +3993,7 @@
         <v>31.536000000000001</v>
       </c>
       <c r="X26" s="1">
-        <v>0.35</v>
+        <v>0.11</v>
       </c>
       <c r="Z26">
         <f>NEMS_EMM_AEO2022!C25+1</f>
@@ -4038,8 +4037,8 @@
         <v>17</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>E_MSW_MSW_01</v>
+        <f t="shared" si="4"/>
+        <v>E_THM_MSW_MSW_01</v>
       </c>
       <c r="C27" t="s">
         <v>211</v>
@@ -4055,7 +4054,7 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="6"/>
-        <v>E_MSW_MSW_01</v>
+        <v>E_THM_MSW_MSW_01</v>
       </c>
       <c r="L27" t="s">
         <v>211</v>

</xml_diff>